<commit_message>
Dodat Drre ĆEVMI user u execu
</commit_message>
<xml_diff>
--- a/testdata/data.xlsx
+++ b/testdata/data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9000"/>
+    <workbookView windowWidth="22188" windowHeight="9000"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="48">
   <si>
     <t>username</t>
   </si>
@@ -168,6 +168,9 @@
   </si>
   <si>
     <t>205-9001021348944-31</t>
+  </si>
+  <si>
+    <t>Drre ĆEVMI</t>
   </si>
 </sst>
 </file>
@@ -1169,14 +1172,14 @@
   <sheetPr/>
   <dimension ref="A1:V6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.87962962962963" defaultRowHeight="14.4" outlineLevelRow="5"/>
   <cols>
     <col min="1" max="1" width="17.75" customWidth="1"/>
-    <col min="2" max="2" width="31" customWidth="1"/>
+    <col min="2" max="2" width="35.5555555555556" customWidth="1"/>
     <col min="3" max="3" width="7.75" customWidth="1"/>
     <col min="4" max="4" width="11.25" customWidth="1"/>
     <col min="5" max="5" width="22.4444444444444" customWidth="1"/>
@@ -1467,12 +1470,33 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" customFormat="1" spans="2:22">
-      <c r="B5" s="5"/>
+    <row r="5" customFormat="1" spans="1:22">
+      <c r="A5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>28</v>
+      </c>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
-      <c r="L5" s="1"/>
+      <c r="K5" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>42</v>
+      </c>
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
@@ -1506,6 +1530,7 @@
     <hyperlink ref="B2" r:id="rId1" display="https://uat.dbp.nlb.si/web-retail/login" tooltip="https://uat.dbp.nlb.si/web-retail/login"/>
     <hyperlink ref="B3" r:id="rId1" display="https://uat.dbp.nlb.si/web-retail/login" tooltip="https://uat.dbp.nlb.si/web-retail/login"/>
     <hyperlink ref="B4" r:id="rId1" display="https://uat.dbp.nlb.si/web-retail/login" tooltip="https://uat.dbp.nlb.si/web-retail/login"/>
+    <hyperlink ref="B5" r:id="rId1" display="https://uat.dbp.nlb.si/web-retail/login" tooltip="https://uat.dbp.nlb.si/web-retail/login"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Popravka Loan i data
</commit_message>
<xml_diff>
--- a/testdata/data.xlsx
+++ b/testdata/data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="22188" windowHeight="9000"/>
+    <workbookView windowWidth="23040" windowHeight="10187"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="49">
   <si>
     <t>username</t>
   </si>
@@ -158,19 +158,22 @@
     <t>205-9001001626239-86</t>
   </si>
   <si>
+    <t>Aor IĆVR</t>
+  </si>
+  <si>
+    <t>205-9001021348944-31</t>
+  </si>
+  <si>
+    <t>Drre ĆEVMI</t>
+  </si>
+  <si>
+    <t>Jail ĆEVGIMILĆ</t>
+  </si>
+  <si>
     <t>205-0049032401456-48</t>
   </si>
   <si>
-    <t>Cash loans</t>
-  </si>
-  <si>
-    <t>Aor IĆVR</t>
-  </si>
-  <si>
-    <t>205-9001021348944-31</t>
-  </si>
-  <si>
-    <t>Drre ĆEVMI</t>
+    <t>Gotovinski kredit</t>
   </si>
 </sst>
 </file>
@@ -214,9 +217,9 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -239,9 +242,9 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -693,10 +696,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
@@ -1172,8 +1175,8 @@
   <sheetPr/>
   <dimension ref="A1:V6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="T10" sqref="T10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.87962962962963" defaultRowHeight="14.4" outlineLevelRow="5"/>
@@ -1390,10 +1393,10 @@
         <v>28</v>
       </c>
       <c r="S3" s="1" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="T3" s="1" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="U3" s="1" t="s">
         <v>28</v>
@@ -1404,7 +1407,7 @@
     </row>
     <row r="4" customFormat="1" spans="1:22">
       <c r="A4" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>23</v>
@@ -1425,7 +1428,7 @@
         <v>41</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>28</v>
@@ -1472,7 +1475,7 @@
     </row>
     <row r="5" customFormat="1" spans="1:22">
       <c r="A5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>23</v>
@@ -1489,41 +1492,116 @@
       <c r="F5" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
+      <c r="I5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="K5" s="1" t="s">
         <v>41</v>
       </c>
       <c r="L5" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="M5" s="1"/>
-      <c r="N5" s="1"/>
-      <c r="O5" s="1"/>
-      <c r="P5" s="1"/>
-      <c r="Q5" s="1"/>
-      <c r="R5" s="1"/>
-      <c r="S5" s="1"/>
-      <c r="T5" s="1"/>
-      <c r="U5" s="1"/>
-      <c r="V5" s="1"/>
+      <c r="M5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="R5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="S5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="T5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="U5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="V5" s="1" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="6" customFormat="1" spans="2:22">
-      <c r="B6" s="5"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-      <c r="K6" s="1"/>
-      <c r="L6" s="1"/>
-      <c r="M6" s="1"/>
-      <c r="N6" s="1"/>
-      <c r="O6" s="1"/>
-      <c r="P6" s="1"/>
-      <c r="Q6" s="1"/>
-      <c r="R6" s="1"/>
-      <c r="S6" s="1"/>
-      <c r="T6" s="1"/>
-      <c r="U6" s="1"/>
-      <c r="V6" s="1"/>
+    <row r="6" s="1" customFormat="1" spans="1:22">
+      <c r="A6" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="R6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="S6" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="T6" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="U6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="V6" s="1" t="s">
+        <v>28</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1531,6 +1609,7 @@
     <hyperlink ref="B3" r:id="rId1" display="https://uat.dbp.nlb.si/web-retail/login" tooltip="https://uat.dbp.nlb.si/web-retail/login"/>
     <hyperlink ref="B4" r:id="rId1" display="https://uat.dbp.nlb.si/web-retail/login" tooltip="https://uat.dbp.nlb.si/web-retail/login"/>
     <hyperlink ref="B5" r:id="rId1" display="https://uat.dbp.nlb.si/web-retail/login" tooltip="https://uat.dbp.nlb.si/web-retail/login"/>
+    <hyperlink ref="B6" r:id="rId1" display="https://uat.dbp.nlb.si/web-retail/login" tooltip="https://uat.dbp.nlb.si/web-retail/login"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Zavrseni Android testovi 23.12.25.
</commit_message>
<xml_diff>
--- a/testdata/data.xlsx
+++ b/testdata/data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9467"/>
+    <workbookView windowWidth="23040" windowHeight="9000"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="49">
   <si>
     <t>username</t>
   </si>
@@ -150,6 +150,9 @@
   </si>
   <si>
     <t>Tekući račun</t>
+  </si>
+  <si>
+    <t>205-9001010537788-94</t>
   </si>
   <si>
     <t>205-9001001626239-86</t>
@@ -1172,8 +1175,12 @@
   <sheetPr/>
   <dimension ref="A1:V6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="Q20" sqref="Q20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+      <selection/>
+      <selection pane="topRight"/>
+      <selection pane="bottomLeft"/>
+      <selection pane="bottomRight" activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.87962962962963" defaultRowHeight="14.4" outlineLevelRow="5"/>
@@ -1357,7 +1364,7 @@
         <v>40</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>28</v>
@@ -1369,7 +1376,7 @@
         <v>40</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="M3" s="1" t="s">
         <v>28</v>
@@ -1404,7 +1411,7 @@
     </row>
     <row r="4" customFormat="1" spans="1:22">
       <c r="A4" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>23</v>
@@ -1425,7 +1432,7 @@
         <v>40</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>28</v>
@@ -1437,7 +1444,7 @@
         <v>40</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="M4" s="1" t="s">
         <v>28</v>
@@ -1472,7 +1479,7 @@
     </row>
     <row r="5" customFormat="1" spans="1:22">
       <c r="A5" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>23</v>
@@ -1499,7 +1506,7 @@
         <v>40</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="M5" s="1" t="s">
         <v>28</v>
@@ -1534,7 +1541,7 @@
     </row>
     <row r="6" s="1" customFormat="1" spans="1:22">
       <c r="A6" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>23</v>
@@ -1555,7 +1562,7 @@
         <v>40</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>28</v>
@@ -1588,10 +1595,10 @@
         <v>28</v>
       </c>
       <c r="S6" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="T6" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="U6" s="1" t="s">
         <v>28</v>

</xml_diff>

<commit_message>
Testovi 15 januar 2026
</commit_message>
<xml_diff>
--- a/testdata/data.xlsx
+++ b/testdata/data.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="54">
   <si>
     <t>username</t>
   </si>
@@ -113,49 +113,52 @@
     <t>uat</t>
   </si>
   <si>
+    <t>9032022325800</t>
+  </si>
+  <si>
+    <t>Oročeni depozit</t>
+  </si>
+  <si>
+    <t>.</t>
+  </si>
+  <si>
+    <t>205-9001007790944-88</t>
+  </si>
+  <si>
+    <t>205-9031004419532-81</t>
+  </si>
+  <si>
+    <t>Foreign currency payment accounts</t>
+  </si>
+  <si>
+    <t>Devizni platni račun</t>
+  </si>
+  <si>
+    <t>205-9031004417882-84</t>
+  </si>
+  <si>
+    <t>Payment account with basic services</t>
+  </si>
+  <si>
+    <t>9011008384007</t>
+  </si>
+  <si>
+    <t>9011008395360</t>
+  </si>
+  <si>
+    <t>Naknada za TR</t>
+  </si>
+  <si>
+    <t>A vista depozitni račun</t>
+  </si>
+  <si>
+    <t>Visa prepaid</t>
+  </si>
+  <si>
+    <t>4431********0118</t>
+  </si>
+  <si>
     <t>205-9032022325800-66</t>
-  </si>
-  <si>
-    <t>Oročeni depozit</t>
-  </si>
-  <si>
-    <t>.</t>
-  </si>
-  <si>
-    <t>205-9001007790944-88</t>
-  </si>
-  <si>
-    <t>205-9031004419532-81</t>
-  </si>
-  <si>
-    <t>Foreign currency payment accounts</t>
-  </si>
-  <si>
-    <t>Devizni platni račun</t>
-  </si>
-  <si>
-    <t>205-9031004417882-84</t>
-  </si>
-  <si>
-    <t>Payment account with basic services</t>
-  </si>
-  <si>
-    <t>9011008384007</t>
-  </si>
-  <si>
-    <t>9011008395360</t>
-  </si>
-  <si>
-    <t>Naknada za TR</t>
-  </si>
-  <si>
-    <t>A vista depozitni račun</t>
-  </si>
-  <si>
-    <t>Visa prepaid</t>
-  </si>
-  <si>
-    <t>4431********0118</t>
   </si>
   <si>
     <t>Enil ČIĆVI</t>
@@ -864,6 +867,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" quotePrefix="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" quotePrefix="1">
@@ -1191,11 +1197,11 @@
   <dimension ref="A1:X6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="O2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="T4" sqref="T4"/>
+      <selection pane="bottomRight" activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.87962962962963" defaultRowHeight="14.4" outlineLevelRow="5"/>
@@ -1307,7 +1313,7 @@
       <c r="D2" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="9" t="s">
         <v>28</v>
       </c>
       <c r="F2" s="1" t="s">
@@ -1337,10 +1343,10 @@
       <c r="N2" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="O2" s="9" t="s">
+      <c r="O2" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="P2" s="9" t="s">
+      <c r="P2" s="10" t="s">
         <v>38</v>
       </c>
       <c r="Q2" s="8" t="s">
@@ -1362,7 +1368,7 @@
         <v>30</v>
       </c>
       <c r="W2" s="8" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="X2" s="8" t="s">
         <v>29</v>
@@ -1370,7 +1376,7 @@
     </row>
     <row r="3" customFormat="1" spans="1:24">
       <c r="A3" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>25</v>
@@ -1388,22 +1394,22 @@
         <v>30</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H3" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K3" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="I3" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="L3" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="M3" s="1" t="s">
         <v>30</v>
@@ -1440,7 +1446,7 @@
     </row>
     <row r="4" customFormat="1" spans="1:24">
       <c r="A4" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>25</v>
@@ -1458,10 +1464,10 @@
         <v>30</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>30</v>
@@ -1470,10 +1476,10 @@
         <v>30</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="M4" s="1" t="s">
         <v>30</v>
@@ -1510,7 +1516,7 @@
     </row>
     <row r="5" customFormat="1" spans="1:24">
       <c r="A5" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>25</v>
@@ -1534,10 +1540,10 @@
         <v>30</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="M5" s="1" t="s">
         <v>30</v>
@@ -1574,7 +1580,7 @@
     </row>
     <row r="6" s="1" customFormat="1" spans="1:24">
       <c r="A6" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>25</v>
@@ -1592,10 +1598,10 @@
         <v>30</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>30</v>
@@ -1628,10 +1634,10 @@
         <v>30</v>
       </c>
       <c r="U6" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="V6" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="W6" s="1" t="s">
         <v>30</v>

</xml_diff>

<commit_message>
Promena data i deposit testovi u Product summary
</commit_message>
<xml_diff>
--- a/testdata/data.xlsx
+++ b/testdata/data.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="60">
   <si>
     <t>username</t>
   </si>
@@ -47,6 +47,15 @@
     <t>termDepositName</t>
   </si>
   <si>
+    <t>term_deposit_account_details_opening_date</t>
+  </si>
+  <si>
+    <t>term_deposit_account_details_expiration_date</t>
+  </si>
+  <si>
+    <t>maturity_account</t>
+  </si>
+  <si>
     <t>currentDomesticAccountName</t>
   </si>
   <si>
@@ -65,12 +74,6 @@
     <t>second_personal_account_bban</t>
   </si>
   <si>
-    <t>third_personal_account_bban</t>
-  </si>
-  <si>
-    <t>third_personal_account_name</t>
-  </si>
-  <si>
     <t>saving_account_bban</t>
   </si>
   <si>
@@ -119,6 +122,12 @@
     <t>Oročeni depozit</t>
   </si>
   <si>
+    <t>15. 1. 2016</t>
+  </si>
+  <si>
+    <t>15. 1. 2028</t>
+  </si>
+  <si>
     <t>.</t>
   </si>
   <si>
@@ -134,10 +143,7 @@
     <t>Devizni platni račun</t>
   </si>
   <si>
-    <t>205-9031004417882-84</t>
-  </si>
-  <si>
-    <t>Payment account with basic services</t>
+    <t>RS35 2059 0310 0441 7882 84</t>
   </si>
   <si>
     <t>9011008384007</t>
@@ -162,6 +168,18 @@
   </si>
   <si>
     <t>Enil ČIĆVI</t>
+  </si>
+  <si>
+    <t>9032030694661</t>
+  </si>
+  <si>
+    <t>8. 6. 2022</t>
+  </si>
+  <si>
+    <t>8. 6. 2028</t>
+  </si>
+  <si>
+    <t>9031008901983</t>
   </si>
   <si>
     <t>Tekući račun</t>
@@ -201,7 +219,7 @@
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="26">
+  <fonts count="27">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -224,27 +242,28 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <name val="Calibri"/>
       <charset val="134"/>
     </font>
@@ -252,6 +271,11 @@
       <sz val="9"/>
       <color theme="1"/>
       <name val="Segoe UI"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
       <charset val="134"/>
     </font>
     <font>
@@ -711,7 +735,7 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -720,128 +744,128 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -854,8 +878,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="6" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="6" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -869,10 +896,16 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" quotePrefix="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" quotePrefix="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="6" applyFont="1" applyFill="1" applyAlignment="1" quotePrefix="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1194,14 +1227,14 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:X6"/>
+  <dimension ref="A1:Y6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F12" sqref="F12"/>
+      <selection pane="bottomRight" activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.87962962962963" defaultRowHeight="14.4" outlineLevelRow="5"/>
@@ -1212,21 +1245,21 @@
     <col min="4" max="4" width="11.25" customWidth="1"/>
     <col min="5" max="5" width="22.4444444444444" customWidth="1"/>
     <col min="6" max="6" width="17.5555555555556" customWidth="1"/>
-    <col min="7" max="7" width="33.8888888888889" customWidth="1"/>
-    <col min="8" max="8" width="28.8888888888889" customWidth="1"/>
-    <col min="9" max="9" width="23.4259259259259" style="1" customWidth="1"/>
-    <col min="10" max="12" width="30.4259259259259" style="1" customWidth="1"/>
-    <col min="13" max="13" width="38" style="1" customWidth="1"/>
-    <col min="14" max="14" width="30.1111111111111" style="1" customWidth="1"/>
-    <col min="15" max="15" width="19.8888888888889" style="1" customWidth="1"/>
-    <col min="16" max="18" width="24.6666666666667" style="1" customWidth="1"/>
-    <col min="19" max="21" width="33.2222222222222" style="1" customWidth="1"/>
-    <col min="22" max="22" width="31.1111111111111" style="1" customWidth="1"/>
-    <col min="23" max="23" width="33.2222222222222" style="1" customWidth="1"/>
-    <col min="24" max="24" width="19.1111111111111" style="1" customWidth="1"/>
+    <col min="7" max="7" width="42.1111111111111" customWidth="1"/>
+    <col min="8" max="8" width="44.1111111111111" customWidth="1"/>
+    <col min="9" max="10" width="33.8888888888889" customWidth="1"/>
+    <col min="11" max="11" width="28.8888888888889" customWidth="1"/>
+    <col min="12" max="12" width="23.4259259259259" style="1" customWidth="1"/>
+    <col min="13" max="15" width="30.4259259259259" style="1" customWidth="1"/>
+    <col min="16" max="16" width="19.8888888888889" style="1" customWidth="1"/>
+    <col min="17" max="19" width="24.6666666666667" style="1" customWidth="1"/>
+    <col min="20" max="22" width="33.2222222222222" style="1" customWidth="1"/>
+    <col min="23" max="23" width="31.1111111111111" style="1" customWidth="1"/>
+    <col min="24" max="24" width="33.2222222222222" style="1" customWidth="1"/>
+    <col min="25" max="25" width="19.1111111111111" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="1" spans="1:24">
+    <row r="1" customFormat="1" spans="1:25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1269,22 +1302,22 @@
       <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="7" t="s">
+      <c r="P1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="7" t="s">
+      <c r="Q1" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="R1" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="7" t="s">
+      <c r="S1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="T1" s="10" t="s">
         <v>19</v>
       </c>
       <c r="U1" s="1" t="s">
@@ -1299,351 +1332,345 @@
       <c r="X1" s="1" t="s">
         <v>23</v>
       </c>
+      <c r="Y1" s="1" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="2" customFormat="1" spans="1:24">
+    <row r="2" customFormat="1" spans="1:25">
       <c r="A2" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E2" s="9" t="s">
         <v>28</v>
       </c>
+      <c r="E2" s="11" t="s">
+        <v>29</v>
+      </c>
       <c r="F2" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="H2" s="4" t="s">
         <v>31</v>
       </c>
+      <c r="H2" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="I2" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="K2" s="8" t="s">
         <v>34</v>
       </c>
       <c r="L2" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="M2" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="N2" s="8" t="s">
+      <c r="M2" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="O2" s="10" t="s">
+      <c r="N2" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="P2" s="10" t="s">
+      <c r="O2" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="Q2" s="8" t="s">
+      <c r="P2" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="R2" s="8" t="s">
+      <c r="Q2" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="S2" s="8" t="s">
+      <c r="R2" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="T2" s="1" t="s">
+      <c r="S2" s="9" t="s">
         <v>42</v>
       </c>
+      <c r="T2" s="9" t="s">
+        <v>43</v>
+      </c>
       <c r="U2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="X2" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="Y2" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="V2" s="1" t="s">
+    </row>
+    <row r="3" customFormat="1" spans="1:25">
+      <c r="A3" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="F3" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="W2" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="X2" s="8" t="s">
-        <v>29</v>
+      <c r="G3" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="I3" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q3" s="1"/>
+      <c r="R3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="T3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="U3" s="1"/>
+      <c r="V3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="W3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="X3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Y3" s="1" t="s">
+        <v>33</v>
       </c>
     </row>
-    <row r="3" customFormat="1" spans="1:24">
-      <c r="A3" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C3" s="2" t="s">
+    <row r="4" customFormat="1" spans="1:25">
+      <c r="A4" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="C4" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E3" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="O3" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="P3" s="1"/>
-      <c r="Q3" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="R3" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="S3" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="T3" s="1"/>
-      <c r="U3" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="V3" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="W3" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="X3" s="1" t="s">
-        <v>30</v>
+      <c r="D4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q4" s="1"/>
+      <c r="R4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="S4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="T4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="U4" s="1"/>
+      <c r="V4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="W4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="X4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Y4" s="1" t="s">
+        <v>33</v>
       </c>
     </row>
-    <row r="4" customFormat="1" spans="1:24">
-      <c r="A4" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C4" s="2" t="s">
+    <row r="5" customFormat="1" spans="1:25">
+      <c r="A5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="C5" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E4" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="M4" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="N4" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="O4" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="P4" s="1"/>
-      <c r="Q4" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="R4" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="S4" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="T4" s="1"/>
-      <c r="U4" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="V4" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="W4" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="X4" s="1" t="s">
-        <v>30</v>
+      <c r="D5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q5" s="1"/>
+      <c r="R5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="S5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="T5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="U5" s="1"/>
+      <c r="V5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="W5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="X5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Y5" s="1" t="s">
+        <v>33</v>
       </c>
     </row>
-    <row r="5" customFormat="1" spans="1:24">
-      <c r="A5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C5" s="2" t="s">
+    <row r="6" s="1" customFormat="1" spans="1:25">
+      <c r="A6" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B6" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="C6" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E5" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="M5" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="N5" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="O5" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="P5" s="1"/>
-      <c r="Q5" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="R5" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="S5" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="T5" s="1"/>
-      <c r="U5" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="V5" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="W5" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="X5" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" s="1" customFormat="1" spans="1:24">
-      <c r="A6" s="1" t="s">
+      <c r="D6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="J6" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B6" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="K6" s="1" t="s">
-        <v>30</v>
+        <v>53</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q6" s="1" t="s">
-        <v>30</v>
+        <v>33</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="R6" s="1" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="S6" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="U6" s="1" t="s">
-        <v>52</v>
+        <v>33</v>
+      </c>
+      <c r="T6" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="V6" s="1" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="W6" s="1" t="s">
-        <v>30</v>
+        <v>59</v>
       </c>
       <c r="X6" s="1" t="s">
-        <v>30</v>
+        <v>33</v>
+      </c>
+      <c r="Y6" s="1" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cards transaction filter custom range i invalid filter
</commit_message>
<xml_diff>
--- a/testdata/data.xlsx
+++ b/testdata/data.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="64">
   <si>
     <t>username</t>
   </si>
@@ -92,6 +92,12 @@
     <t>credit_card_number</t>
   </si>
   <si>
+    <t>credit_card_2_name</t>
+  </si>
+  <si>
+    <t>credit_card_2_number</t>
+  </si>
+  <si>
     <t>loan_account_bban</t>
   </si>
   <si>
@@ -162,6 +168,12 @@
   </si>
   <si>
     <t>4431********0118</t>
+  </si>
+  <si>
+    <t>Visa revolving card</t>
+  </si>
+  <si>
+    <t>4176********8476</t>
   </si>
   <si>
     <t>205-9032022325800-66</t>
@@ -1227,14 +1239,14 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:Y6"/>
+  <dimension ref="A1:AA6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="S2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="K1" sqref="K1"/>
+      <selection pane="bottomRight" activeCell="W5" sqref="W5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.87962962962963" defaultRowHeight="14.4" outlineLevelRow="5"/>
@@ -1253,13 +1265,13 @@
     <col min="13" max="15" width="30.4259259259259" style="1" customWidth="1"/>
     <col min="16" max="16" width="19.8888888888889" style="1" customWidth="1"/>
     <col min="17" max="19" width="24.6666666666667" style="1" customWidth="1"/>
-    <col min="20" max="22" width="33.2222222222222" style="1" customWidth="1"/>
-    <col min="23" max="23" width="31.1111111111111" style="1" customWidth="1"/>
-    <col min="24" max="24" width="33.2222222222222" style="1" customWidth="1"/>
-    <col min="25" max="25" width="19.1111111111111" style="1" customWidth="1"/>
+    <col min="20" max="24" width="33.2222222222222" style="1" customWidth="1"/>
+    <col min="25" max="25" width="31.1111111111111" style="1" customWidth="1"/>
+    <col min="26" max="26" width="33.2222222222222" style="1" customWidth="1"/>
+    <col min="27" max="27" width="19.1111111111111" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="1" spans="1:25">
+    <row r="1" customFormat="1" spans="1:27">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1335,342 +1347,360 @@
       <c r="Y1" s="1" t="s">
         <v>24</v>
       </c>
+      <c r="Z1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="2" customFormat="1" spans="1:25">
+    <row r="2" customFormat="1" spans="1:27">
       <c r="A2" s="2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="K2" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="P2" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q2" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="R2" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="S2" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="T2" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Y2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Z2" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="AA2" s="9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" customFormat="1" spans="1:27">
+      <c r="A3" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="C3" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="D3" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="H2" s="1" t="s">
+      <c r="E3" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="F3" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="I2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="K2" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="P2" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q2" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="R2" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="S2" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="T2" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="U2" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="V2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="W2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="X2" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="Y2" s="9" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" customFormat="1" spans="1:25">
-      <c r="A3" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E3" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>30</v>
-      </c>
       <c r="G3" s="5" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="I3" s="11" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="Q3" s="1"/>
       <c r="R3" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="S3" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="T3" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="U3" s="1"/>
-      <c r="V3" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="W3" s="1" t="s">
-        <v>33</v>
-      </c>
+      <c r="V3" s="1"/>
+      <c r="W3" s="1"/>
       <c r="X3" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="Y3" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
+      </c>
+      <c r="Z3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AA3" s="1" t="s">
+        <v>35</v>
       </c>
     </row>
-    <row r="4" customFormat="1" spans="1:25">
+    <row r="4" customFormat="1" spans="1:27">
       <c r="A4" s="1" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="K4" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="N4" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="L4" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="M4" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="N4" s="1" t="s">
-        <v>51</v>
-      </c>
       <c r="O4" s="1" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="Q4" s="1"/>
       <c r="R4" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="S4" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="T4" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="U4" s="1"/>
-      <c r="V4" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="W4" s="1" t="s">
-        <v>33</v>
-      </c>
+      <c r="V4" s="1"/>
+      <c r="W4" s="1"/>
       <c r="X4" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="Y4" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
+      </c>
+      <c r="Z4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AA4" s="1" t="s">
+        <v>35</v>
       </c>
     </row>
-    <row r="5" customFormat="1" spans="1:25">
+    <row r="5" customFormat="1" spans="1:27">
       <c r="A5" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="Q5" s="1"/>
       <c r="R5" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="S5" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="T5" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="U5" s="1"/>
-      <c r="V5" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="W5" s="1" t="s">
-        <v>33</v>
-      </c>
+      <c r="V5" s="1"/>
+      <c r="W5" s="1"/>
       <c r="X5" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="Y5" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
+      </c>
+      <c r="Z5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AA5" s="1" t="s">
+        <v>35</v>
       </c>
     </row>
-    <row r="6" s="1" customFormat="1" spans="1:25">
+    <row r="6" s="1" customFormat="1" spans="1:27">
       <c r="A6" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="K6" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B6" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>53</v>
-      </c>
       <c r="L6" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="R6" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="S6" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="T6" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="V6" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="W6" s="1" t="s">
-        <v>59</v>
+        <v>35</v>
       </c>
       <c r="X6" s="1" t="s">
-        <v>33</v>
+        <v>62</v>
       </c>
       <c r="Y6" s="1" t="s">
-        <v>33</v>
+        <v>63</v>
+      </c>
+      <c r="Z6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AA6" s="1" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
prepravke prije pustanja 6.2.2026.
</commit_message>
<xml_diff>
--- a/testdata/data.xlsx
+++ b/testdata/data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="22188" windowHeight="9000"/>
+    <workbookView windowWidth="23040" windowHeight="10187"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="68">
   <si>
     <t>username</t>
   </si>
@@ -74,6 +74,9 @@
     <t>second_personal_account_bban</t>
   </si>
   <si>
+    <t>second_personal_account_iban</t>
+  </si>
+  <si>
     <t>saving_account_bban</t>
   </si>
   <si>
@@ -137,6 +140,9 @@
     <t>.</t>
   </si>
   <si>
+    <t>Tekući račun</t>
+  </si>
+  <si>
     <t>205-9001007790944-88</t>
   </si>
   <si>
@@ -149,6 +155,9 @@
     <t>Devizni platni račun</t>
   </si>
   <si>
+    <t>205-9031004417882-84</t>
+  </si>
+  <si>
     <t>RS35 2059 0310 0441 7882 84</t>
   </si>
   <si>
@@ -194,9 +203,6 @@
     <t>9031008901983</t>
   </si>
   <si>
-    <t>Tekući račun</t>
-  </si>
-  <si>
     <t>205-9001010537788-94</t>
   </si>
   <si>
@@ -213,6 +219,9 @@
   </si>
   <si>
     <t>Drre ĆEVMI</t>
+  </si>
+  <si>
+    <t>205-9001007839862-95</t>
   </si>
   <si>
     <t>Jail ĆEVGIMILĆ</t>
@@ -283,14 +292,14 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+    </font>
+    <font>
       <sz val="9"/>
       <color theme="1"/>
       <name val="Segoe UI"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
       <charset val="134"/>
     </font>
     <font>
@@ -917,7 +926,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" quotePrefix="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" quotePrefix="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" quotePrefix="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="6" applyFont="1" applyFill="1" applyAlignment="1" quotePrefix="1">
@@ -1242,14 +1251,14 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:AA6"/>
+  <dimension ref="A1:AB6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="L2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="K1" sqref="K1"/>
+      <selection pane="bottomRight" activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.87962962962963" defaultRowHeight="14.4" outlineLevelRow="5"/>
@@ -1266,15 +1275,15 @@
     <col min="11" max="11" width="28.8888888888889" customWidth="1"/>
     <col min="12" max="12" width="27.8888888888889" style="1" customWidth="1"/>
     <col min="13" max="15" width="30.4259259259259" style="1" customWidth="1"/>
-    <col min="16" max="16" width="19.8888888888889" style="1" customWidth="1"/>
-    <col min="17" max="19" width="24.6666666666667" style="1" customWidth="1"/>
-    <col min="20" max="24" width="33.2222222222222" style="1" customWidth="1"/>
-    <col min="25" max="25" width="31.1111111111111" style="1" customWidth="1"/>
-    <col min="26" max="26" width="33.2222222222222" style="1" customWidth="1"/>
-    <col min="27" max="27" width="19.1111111111111" style="1" customWidth="1"/>
+    <col min="16" max="17" width="19.8888888888889" style="1" customWidth="1"/>
+    <col min="18" max="20" width="24.6666666666667" style="1" customWidth="1"/>
+    <col min="21" max="25" width="33.2222222222222" style="1" customWidth="1"/>
+    <col min="26" max="26" width="31.1111111111111" style="1" customWidth="1"/>
+    <col min="27" max="27" width="33.2222222222222" style="1" customWidth="1"/>
+    <col min="28" max="28" width="19.1111111111111" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="1" spans="1:27">
+    <row r="1" customFormat="1" spans="1:28">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1320,22 +1329,22 @@
       <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="P1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="10" t="s">
+      <c r="Q1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="10" t="s">
+      <c r="R1" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="S1" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="10" t="s">
+      <c r="T1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="U1" s="9" t="s">
         <v>20</v>
       </c>
       <c r="V1" s="1" t="s">
@@ -1356,354 +1365,375 @@
       <c r="AA1" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="AB1" s="1" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="2" customFormat="1" spans="1:27">
+    <row r="2" customFormat="1" spans="1:28">
       <c r="A2" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K2" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q2" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="R2" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="S2" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="T2" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="U2" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA2" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="AB2" s="10" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" customFormat="1" spans="1:28">
+      <c r="A3" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="D3" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="G2" s="1" t="s">
+      <c r="E3" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="F3" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="H2" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="K2" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="L2" s="1" t="s">
+      <c r="G3" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I3" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="J3" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="M2" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="P2" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q2" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="R2" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="S2" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="T2" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="U2" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="V2" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="W2" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="X2" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="Y2" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="Z2" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="AA2" s="9" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="3" customFormat="1" spans="1:27">
-      <c r="A3" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E3" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="I3" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>55</v>
-      </c>
       <c r="K3" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>55</v>
+        <v>37</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>57</v>
+        <v>36</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q3" s="1"/>
-      <c r="R3" s="1" t="s">
-        <v>35</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="R3" s="1"/>
       <c r="S3" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="T3" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="U3" s="1"/>
+        <v>36</v>
+      </c>
+      <c r="U3" s="1" t="s">
+        <v>36</v>
+      </c>
       <c r="V3" s="1"/>
       <c r="W3" s="1"/>
-      <c r="X3" s="1" t="s">
-        <v>35</v>
-      </c>
+      <c r="X3" s="1"/>
       <c r="Y3" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="Z3" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="AA3" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
+      </c>
+      <c r="AB3" s="1" t="s">
+        <v>36</v>
       </c>
     </row>
-    <row r="4" customFormat="1" spans="1:27">
+    <row r="4" customFormat="1" spans="1:28">
       <c r="A4" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1" t="s">
-        <v>55</v>
+        <v>37</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>55</v>
+        <v>37</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q4" s="1"/>
-      <c r="R4" s="1" t="s">
-        <v>35</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="R4" s="1"/>
       <c r="S4" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="T4" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="U4" s="1"/>
+        <v>36</v>
+      </c>
+      <c r="U4" s="1" t="s">
+        <v>36</v>
+      </c>
       <c r="V4" s="1"/>
       <c r="W4" s="1"/>
-      <c r="X4" s="1" t="s">
-        <v>35</v>
-      </c>
+      <c r="X4" s="1"/>
       <c r="Y4" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="Z4" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="AA4" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
+      </c>
+      <c r="AB4" s="1" t="s">
+        <v>36</v>
       </c>
     </row>
-    <row r="5" customFormat="1" spans="1:27">
+    <row r="5" customFormat="1" spans="1:28">
       <c r="A5" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>35</v>
+        <v>36</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>64</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>55</v>
+        <v>37</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q5" s="1"/>
-      <c r="R5" s="1" t="s">
-        <v>35</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="R5" s="1"/>
       <c r="S5" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="T5" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="U5" s="1"/>
+        <v>36</v>
+      </c>
+      <c r="U5" s="1" t="s">
+        <v>36</v>
+      </c>
       <c r="V5" s="1"/>
       <c r="W5" s="1"/>
-      <c r="X5" s="1" t="s">
-        <v>35</v>
-      </c>
+      <c r="X5" s="1"/>
       <c r="Y5" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="Z5" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="AA5" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
+      </c>
+      <c r="AB5" s="1" t="s">
+        <v>36</v>
       </c>
     </row>
-    <row r="6" s="1" customFormat="1" spans="1:27">
+    <row r="6" s="1" customFormat="1" spans="1:28">
       <c r="A6" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K6" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B6" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>60</v>
-      </c>
       <c r="L6" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="P6" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="R6" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
+      </c>
+      <c r="Q6" s="1" t="s">
+        <v>36</v>
       </c>
       <c r="S6" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="T6" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="X6" s="1" t="s">
-        <v>63</v>
+        <v>36</v>
+      </c>
+      <c r="U6" s="1" t="s">
+        <v>36</v>
       </c>
       <c r="Y6" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="Z6" s="1" t="s">
-        <v>35</v>
+        <v>67</v>
       </c>
       <c r="AA6" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
+      </c>
+      <c r="AB6" s="1" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
izmjene i pustanje 6. februar
</commit_message>
<xml_diff>
--- a/testdata/data.xlsx
+++ b/testdata/data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="10187"/>
+    <workbookView windowWidth="23040" windowHeight="9467"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="68">
   <si>
     <t>username</t>
   </si>
@@ -1254,11 +1254,11 @@
   <dimension ref="A1:AB6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="L2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="O2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="O2" sqref="O2"/>
+      <selection pane="bottomRight" activeCell="Q11" sqref="Q11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.87962962962963" defaultRowHeight="14.4" outlineLevelRow="5"/>
@@ -1275,7 +1275,8 @@
     <col min="11" max="11" width="28.8888888888889" customWidth="1"/>
     <col min="12" max="12" width="27.8888888888889" style="1" customWidth="1"/>
     <col min="13" max="15" width="30.4259259259259" style="1" customWidth="1"/>
-    <col min="16" max="17" width="19.8888888888889" style="1" customWidth="1"/>
+    <col min="16" max="16" width="44.5555555555556" style="1" customWidth="1"/>
+    <col min="17" max="17" width="19.8888888888889" style="1" customWidth="1"/>
     <col min="18" max="20" width="24.6666666666667" style="1" customWidth="1"/>
     <col min="21" max="25" width="33.2222222222222" style="1" customWidth="1"/>
     <col min="26" max="26" width="31.1111111111111" style="1" customWidth="1"/>
@@ -1507,7 +1508,9 @@
       <c r="Q3" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="R3" s="1"/>
+      <c r="R3" s="1" t="s">
+        <v>36</v>
+      </c>
       <c r="S3" s="1" t="s">
         <v>36</v>
       </c>
@@ -1579,7 +1582,9 @@
       <c r="Q4" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="R4" s="1"/>
+      <c r="R4" s="1" t="s">
+        <v>36</v>
+      </c>
       <c r="S4" s="1" t="s">
         <v>36</v>
       </c>
@@ -1648,7 +1653,9 @@
       <c r="Q5" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="R5" s="1"/>
+      <c r="R5" s="1" t="s">
+        <v>36</v>
+      </c>
       <c r="S5" s="1" t="s">
         <v>36</v>
       </c>
@@ -1712,6 +1719,9 @@
         <v>36</v>
       </c>
       <c r="Q6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="R6" s="1" t="s">
         <v>36</v>
       </c>
       <c r="S6" s="1" t="s">

</xml_diff>